<commit_message>
topsis working on gui
</commit_message>
<xml_diff>
--- a/lab-4/data.xlsx
+++ b/lab-4/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomis\Desktop\OW\multicriteria-optimization\lab-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD4963BC-3A76-41CB-807F-28C220AB4B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642F6124-F15B-449E-AFDB-F3C4FFBA0EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F6F971CA-CF19-442E-8710-D557B73709E3}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F6F971CA-CF19-442E-8710-D557B73709E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,10 +151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,18 +491,18 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +519,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -531,16 +527,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>1.7286562823678353E-2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3.9071958857615376</v>
-      </c>
-      <c r="E2" s="2">
-        <v>32.572894994256799</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1">
+        <v>82</v>
+      </c>
+      <c r="E2" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -548,16 +544,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>0.41101967983651222</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3.9244061773452907</v>
-      </c>
-      <c r="E3" s="2">
-        <v>37.949031365019472</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1">
+        <v>64</v>
+      </c>
+      <c r="E3" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -565,16 +561,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>0.61109848036068959</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.75995789480187148</v>
-      </c>
-      <c r="E4" s="2">
-        <v>9.4624004943447346</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1">
+        <v>83</v>
+      </c>
+      <c r="E4" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -582,16 +578,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>0.1919331858321256</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5.0276598854819561</v>
-      </c>
-      <c r="E5" s="2">
-        <v>20.732526374368511</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="D5" s="1">
+        <v>79</v>
+      </c>
+      <c r="E5" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -599,16 +595,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>0.65713031770326269</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4.2441576329110919</v>
-      </c>
-      <c r="E6" s="2">
-        <v>26.190618412118489</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="D6" s="1">
+        <v>80</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -616,16 +612,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>0.14790861462172888</v>
-      </c>
-      <c r="D7" s="2">
-        <v>7.5338579456955381</v>
-      </c>
-      <c r="E7" s="2">
-        <v>6.0267461648626774</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1">
+        <v>71</v>
+      </c>
+      <c r="E7" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -633,16 +629,16 @@
         <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>0.44306512539264342</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5.6661054836455014</v>
-      </c>
-      <c r="E8" s="2">
-        <v>26.876659947024315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="D8" s="1">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -650,16 +646,16 @@
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>0.20200930985133148</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.2358547690865718</v>
-      </c>
-      <c r="E9" s="2">
-        <v>35.175525174256748</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="D9" s="1">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -667,16 +663,16 @@
         <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>0.62081443899290345</v>
-      </c>
-      <c r="D10" s="2">
-        <v>7.3035151576920851</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5.377022607904216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -684,16 +680,16 @@
         <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>0.38572526111062455</v>
-      </c>
-      <c r="D11" s="2">
-        <v>9.2063306432156562</v>
-      </c>
-      <c r="E11" s="2">
-        <v>39.859609704786479</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -701,16 +697,16 @@
         <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>0.52603522680040393</v>
-      </c>
-      <c r="D12" s="2">
-        <v>7.1738661192939848</v>
-      </c>
-      <c r="E12" s="2">
-        <v>24.601836520656164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -718,16 +714,16 @@
         <v>13</v>
       </c>
       <c r="C13" s="1">
-        <v>0.92634457185238084</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2.1257949394414446</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.8393740659249458</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1">
+        <v>67</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -735,16 +731,16 @@
         <v>14</v>
       </c>
       <c r="C14" s="1">
-        <v>0.92136738929945805</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1.5623087138679526</v>
-      </c>
-      <c r="E14" s="2">
-        <v>16.619242685652953</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -752,16 +748,16 @@
         <v>15</v>
       </c>
       <c r="C15" s="1">
-        <v>0.83181512335608165</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5.2800368373751976</v>
-      </c>
-      <c r="E15" s="2">
-        <v>6.0377808748719941</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="D15" s="1">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -769,16 +765,16 @@
         <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>0.84071808371942947</v>
-      </c>
-      <c r="D16" s="2">
-        <v>2.7383564288849573</v>
-      </c>
-      <c r="E16" s="2">
-        <v>10.923548298525594</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="D16" s="1">
+        <v>29</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -786,16 +782,16 @@
         <v>17</v>
       </c>
       <c r="C17" s="1">
-        <v>3.1472453549804102E-2</v>
-      </c>
-      <c r="D17" s="2">
-        <v>6.3874894448262678</v>
-      </c>
-      <c r="E17" s="2">
-        <v>26.217130966468247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -803,16 +799,16 @@
         <v>18</v>
       </c>
       <c r="C18" s="1">
-        <v>0.12653376517038628</v>
-      </c>
-      <c r="D18" s="2">
-        <v>2.6391363907644019</v>
-      </c>
-      <c r="E18" s="2">
-        <v>22.018947746896185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="D18" s="1">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -820,16 +816,16 @@
         <v>19</v>
       </c>
       <c r="C19" s="1">
-        <v>9.4155742023005029E-2</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1.0896827153825783</v>
-      </c>
-      <c r="E19" s="2">
-        <v>33.029994009649869</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1">
+        <v>82</v>
+      </c>
+      <c r="E19" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -837,16 +833,16 @@
         <v>20</v>
       </c>
       <c r="C20" s="1">
-        <v>0.96624919267406117</v>
-      </c>
-      <c r="D20" s="2">
-        <v>9.1998188453205891</v>
-      </c>
-      <c r="E20" s="2">
-        <v>13.758760451693725</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -854,13 +850,13 @@
         <v>21</v>
       </c>
       <c r="C21" s="1">
-        <v>0.82980834101998491</v>
-      </c>
-      <c r="D21" s="2">
-        <v>4.9041644626310008</v>
-      </c>
-      <c r="E21" s="2">
-        <v>23.811740708043033</v>
+        <v>27</v>
+      </c>
+      <c r="D21" s="1">
+        <v>86</v>
+      </c>
+      <c r="E21" s="1">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>